<commit_message>
Keep several test in one file on different sheets.
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\excel-tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C850994-6A5D-4B60-A1CD-F5A81B9D873E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E742BB1-BBE3-4EE8-B8F7-A30A08C3C11C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="test1" sheetId="1" r:id="rId1"/>
+    <sheet name="test2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,19 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>She does not cry when she is upset.</t>
-  </si>
-  <si>
-    <t>Она не плачет, когда она расстроена.</t>
-  </si>
-  <si>
-    <t>I like your dog. What is its name?</t>
-  </si>
-  <si>
-    <t>Мне нравится твоя собака. Как её зовут?</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>question</t>
   </si>
@@ -46,6 +35,21 @@
   </si>
   <si>
     <t>2+2</t>
+  </si>
+  <si>
+    <t>3+2</t>
+  </si>
+  <si>
+    <t>6+3</t>
+  </si>
+  <si>
+    <t>1+1</t>
+  </si>
+  <si>
+    <t>1+2</t>
+  </si>
+  <si>
+    <t>1+3</t>
   </si>
 </sst>
 </file>
@@ -87,11 +91,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -377,44 +378,92 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="37" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
         <v>4</v>
       </c>
-      <c r="B1" s="2" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D6AA3BF-AC16-4D5D-8DC4-C3C38937182F}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
         <v>4</v>
       </c>
     </row>

</xml_diff>